<commit_message>
Updated the framework with buy a product test
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/Testdata.xlsx
+++ b/src/test/resources/excel/Testdata.xlsx
@@ -5,11 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="TestSuite" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="LoginTest" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="BuyProductTest" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="TestSuite" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="LoginTest" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -21,7 +22,70 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="25">
+  <si>
+    <t xml:space="preserve">username</t>
+  </si>
+  <si>
+    <t xml:space="preserve">password</t>
+  </si>
+  <si>
+    <t xml:space="preserve">firstName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lastName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">postalCode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">runmode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">standard_user</t>
+  </si>
+  <si>
+    <t xml:space="preserve">secret_sauce</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anand</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kumar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Y</t>
+  </si>
+  <si>
+    <t xml:space="preserve">locked_out_user</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Balaji</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tester</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N</t>
+  </si>
+  <si>
+    <t xml:space="preserve">problem_user</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chandrasekhar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reddy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">performance_glitch_user</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Damodhar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">prasad</t>
+  </si>
   <si>
     <t xml:space="preserve">TC_ID</t>
   </si>
@@ -32,31 +96,7 @@
     <t xml:space="preserve">LoginTest</t>
   </si>
   <si>
-    <t xml:space="preserve">Y</t>
-  </si>
-  <si>
-    <t xml:space="preserve">username</t>
-  </si>
-  <si>
-    <t xml:space="preserve">password</t>
-  </si>
-  <si>
-    <t xml:space="preserve">runmode</t>
-  </si>
-  <si>
-    <t xml:space="preserve">standard_user</t>
-  </si>
-  <si>
-    <t xml:space="preserve">secret_sauce</t>
-  </si>
-  <si>
-    <t xml:space="preserve">locked_out_user</t>
-  </si>
-  <si>
-    <t xml:space="preserve">problem_user</t>
-  </si>
-  <si>
-    <t xml:space="preserve">performance_glitch_user</t>
+    <t xml:space="preserve">BuyProductTest</t>
   </si>
 </sst>
 </file>
@@ -66,7 +106,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -88,6 +128,20 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="10.5"/>
+      <color rgb="FF9876AA"/>
+      <name val="JetBrains Mono"/>
+      <family val="3"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10.5"/>
+      <color rgb="FF6A8759"/>
+      <name val="JetBrains Mono"/>
+      <family val="3"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -132,12 +186,20 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -150,6 +212,66 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF6A8759"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF9876AA"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -158,31 +280,120 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="8.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="10.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="8.85"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>3</v>
+        <v>7</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="1" t="n">
+        <v>560001</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="1" t="n">
+        <v>560033</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="1" t="n">
+        <v>517505</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" s="1" t="n">
+        <v>517501</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -201,13 +412,65 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.07"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.05"/>
@@ -216,57 +479,57 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="0" t="s">
         <v>5</v>
-      </c>
-      <c r="C1" s="0" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="0" t="s">
         <v>10</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="0" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>